<commit_message>
images for the presentation
</commit_message>
<xml_diff>
--- a/compare_alphabeta_heuristics.xlsx
+++ b/compare_alphabeta_heuristics.xlsx
@@ -99,7 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,16 +107,78 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -124,15 +186,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="8">
+    <cellStyle name="20 % - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="20 % - Accent2" xfId="4" builtinId="34"/>
+    <cellStyle name="20 % - Accent3" xfId="5" builtinId="38"/>
+    <cellStyle name="20 % - Accent4" xfId="6" builtinId="42"/>
+    <cellStyle name="20 % - Accent6" xfId="7" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
+    <cellStyle name="Sortie" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -434,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -773,141 +881,144 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="B11" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
+      <c r="A13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" t="s">
+      <c r="A16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>